<commit_message>
all it tests in package it emx files in package emx add tests: 1. self references 2. tags
</commit_message>
<xml_diff>
--- a/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_deep_nesting.xlsx
+++ b/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_deep_nesting.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="686"/>
+    <workbookView xWindow="5680" yWindow="2300" windowWidth="25600" windowHeight="14600" tabRatio="955"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
-    <sheet name="deep_advanced_TestEntity_1" sheetId="4" r:id="rId4"/>
-    <sheet name="deep_advanced_p_TestEntity_2" sheetId="5" r:id="rId5"/>
-    <sheet name="deep_TestCategorical_1" sheetId="6" r:id="rId6"/>
-    <sheet name="deep_TestXref_1" sheetId="7" r:id="rId7"/>
-    <sheet name="deep_TestXref_2" sheetId="9" r:id="rId8"/>
-    <sheet name="deep_TestMref_1" sheetId="8" r:id="rId9"/>
+    <sheet name="it_deep_advanced_TestEntity_1" sheetId="4" r:id="rId4"/>
+    <sheet name="it_deep_advanced_p_TestEntity_2" sheetId="5" r:id="rId5"/>
+    <sheet name="it_deep_TestCategorical_1" sheetId="6" r:id="rId6"/>
+    <sheet name="it_deep_TestXref_1" sheetId="7" r:id="rId7"/>
+    <sheet name="it_deep_TestXref_2" sheetId="9" r:id="rId8"/>
+    <sheet name="it_deep_TestMref_1" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="461">
   <si>
     <t>name</t>
   </si>
@@ -1379,34 +1379,37 @@
     <t>mref_50,mref_1</t>
   </si>
   <si>
-    <t>deep</t>
-  </si>
-  <si>
-    <t>deep_advanced</t>
-  </si>
-  <si>
-    <t>deep_TestEntity_0</t>
-  </si>
-  <si>
-    <t>deep_advanced_TestEntity_1</t>
-  </si>
-  <si>
-    <t>deep_TestCategorical_1</t>
-  </si>
-  <si>
-    <t>deep_TestXref_1</t>
-  </si>
-  <si>
-    <t>deep_TestXref_2</t>
-  </si>
-  <si>
-    <t>deep_TestMref_1</t>
-  </si>
-  <si>
-    <t>deep_advanced_p</t>
-  </si>
-  <si>
-    <t>deep_advanced_p_TestEntity_2</t>
+    <t>it</t>
+  </si>
+  <si>
+    <t>it_deep</t>
+  </si>
+  <si>
+    <t>it_deep_advanced</t>
+  </si>
+  <si>
+    <t>it_deep_advanced_p</t>
+  </si>
+  <si>
+    <t>it_deep_TestEntity_0</t>
+  </si>
+  <si>
+    <t>it_deep_advanced_TestEntity_1</t>
+  </si>
+  <si>
+    <t>it_deep_advanced_p_TestEntity_2</t>
+  </si>
+  <si>
+    <t>it_deep_TestCategorical_1</t>
+  </si>
+  <si>
+    <t>it_deep_TestXref_1</t>
+  </si>
+  <si>
+    <t>it_deep_TestXref_2</t>
+  </si>
+  <si>
+    <t>it_deep_TestMref_1</t>
   </si>
 </sst>
 </file>
@@ -1462,8 +1465,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1604,7 +1613,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1672,6 +1681,9 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1739,6 +1751,9 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2073,16 +2088,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2098,28 +2114,33 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C3" t="s">
         <v>451</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>450</v>
       </c>
     </row>
@@ -2139,14 +2160,14 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2171,7 +2192,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -2182,13 +2203,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2196,10 +2217,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="E4" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2207,7 +2228,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2215,7 +2236,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2223,7 +2244,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2231,7 +2252,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -2249,15 +2270,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
@@ -2296,7 +2317,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -2310,7 +2331,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C3" t="s">
         <v>136</v>
@@ -2327,7 +2348,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -2344,13 +2365,13 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -2364,13 +2385,13 @@
         <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C6" t="s">
         <v>133</v>
       </c>
       <c r="D6" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -2384,7 +2405,7 @@
         <v>138</v>
       </c>
       <c r="B7" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C7" t="s">
         <v>239</v>
@@ -2401,13 +2422,13 @@
         <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C8" t="s">
         <v>134</v>
       </c>
       <c r="D8" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -2421,7 +2442,7 @@
         <v>394</v>
       </c>
       <c r="B9" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C9" t="s">
         <v>397</v>
@@ -2438,13 +2459,13 @@
         <v>395</v>
       </c>
       <c r="B10" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -2461,7 +2482,7 @@
         <v>396</v>
       </c>
       <c r="B11" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C11" t="s">
         <v>239</v>
@@ -2481,7 +2502,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -2498,7 +2519,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C13" t="s">
         <v>136</v>
@@ -2515,7 +2536,7 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -2529,7 +2550,7 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C15" t="s">
         <v>135</v>
@@ -2546,13 +2567,13 @@
         <v>137</v>
       </c>
       <c r="B16" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -2566,7 +2587,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -2580,13 +2601,13 @@
         <v>240</v>
       </c>
       <c r="B18" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="C18" t="s">
         <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -2600,7 +2621,7 @@
         <v>342</v>
       </c>
       <c r="B19" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="C19" t="s">
         <v>239</v>
@@ -2617,7 +2638,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="C20" t="s">
         <v>136</v>
@@ -2634,13 +2655,13 @@
         <v>241</v>
       </c>
       <c r="B21" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="C21" t="s">
         <v>134</v>
       </c>
       <c r="D21" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -2665,7 +2686,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5648,7 +5669,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6233,7 +6254,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>